<commit_message>
Added storage bucket file processing + incorporated it in the end sequence
</commit_message>
<xml_diff>
--- a/ExitSequence/CurrentSeq.xlsx
+++ b/ExitSequence/CurrentSeq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ckat\Documents\UiPath\P2Main\Team1EmptyString-P2\ExitSequence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644C6C73-354A-4750-99B4-456912C27437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC83DDEE-B9BF-46F2-9AC9-9780717130A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9435" yWindow="1155" windowWidth="14550" windowHeight="10740" xr2:uid="{A13E0E18-C340-46B8-9424-F81A17081BB9}"/>
+    <workbookView xWindow="13455" yWindow="1155" windowWidth="14550" windowHeight="10740" xr2:uid="{A13E0E18-C340-46B8-9424-F81A17081BB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,22 +51,22 @@
     <t>Time Spent</t>
   </si>
   <si>
-    <t>00:16:36</t>
-  </si>
-  <si>
     <t>Twitter</t>
   </si>
   <si>
-    <t>00:37:14</t>
-  </si>
-  <si>
-    <t>00:08:56</t>
-  </si>
-  <si>
-    <t>06:00:31</t>
-  </si>
-  <si>
     <t>Photoshop</t>
+  </si>
+  <si>
+    <t>00:40:11</t>
+  </si>
+  <si>
+    <t>00:26:56</t>
+  </si>
+  <si>
+    <t>00:01:56</t>
+  </si>
+  <si>
+    <t>06:03:31</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,10 +446,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44169</v>
+        <v>44177</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -457,35 +457,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44169</v>
+        <v>44177</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44169</v>
+        <v>44177</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>44169</v>
+        <v>44177</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>